<commit_message>
fixed the wrong label
</commit_message>
<xml_diff>
--- a/results/Performance_analysis.xlsx
+++ b/results/Performance_analysis.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="ne mogu stvarno ne znam de mi n" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="tabela1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -423,7 +423,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle count="3" pivot="0" name="ne mogu stvarno ne znam de mi n-style">
+    <tableStyle count="3" pivot="0" name="tabela1-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
@@ -449,7 +449,7 @@
     <tableColumn name="Max (ms)" id="8"/>
     <tableColumn name="Propusnost (Throughput)" id="9"/>
   </tableColumns>
-  <tableStyleInfo name="ne mogu stvarno ne znam de mi n-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="tabela1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 

</xml_diff>